<commit_message>
data set actualization and minor errors corrected
</commit_message>
<xml_diff>
--- a/content/data/Library_Usage_Small.xlsx
+++ b/content/data/Library_Usage_Small.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="42">
+  <si>
+    <t>Unnamed: 0</t>
+  </si>
   <si>
     <t>Patron Type Code</t>
   </si>
@@ -58,46 +61,79 @@
     <t>Within San Francisco County</t>
   </si>
   <si>
+    <t>Teen</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t>Senior</t>
+  </si>
+  <si>
     <t>Juvenile</t>
   </si>
   <si>
-    <t>Teen</t>
-  </si>
-  <si>
-    <t>Adult</t>
+    <t>10 to 19 years</t>
+  </si>
+  <si>
+    <t>25 to 34 years</t>
+  </si>
+  <si>
+    <t>20 to 24 years</t>
+  </si>
+  <si>
+    <t>75 years and over</t>
+  </si>
+  <si>
+    <t>45 to 54 years</t>
   </si>
   <si>
     <t>0 to 9 years</t>
   </si>
   <si>
-    <t>10 to 19 years</t>
-  </si>
-  <si>
-    <t>35 to 44 years</t>
-  </si>
-  <si>
-    <t>r3</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
-    <t>m4</t>
-  </si>
-  <si>
-    <t>b2</t>
-  </si>
-  <si>
-    <t>Richmond</t>
+    <t>p9</t>
+  </si>
+  <si>
+    <t>yb</t>
+  </si>
+  <si>
+    <t>m2</t>
   </si>
   <si>
     <t>Main</t>
   </si>
   <si>
-    <t>Merced</t>
-  </si>
-  <si>
-    <t>Bayview</t>
+    <t>Presidio</t>
+  </si>
+  <si>
+    <t>Bookmobile</t>
+  </si>
+  <si>
+    <t>Marina</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
   </si>
   <si>
     <t>z</t>
@@ -461,13 +497,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,384 +546,474 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
+        <v>123022</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>17</v>
+      <c r="E2">
+        <v>0</v>
       </c>
       <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2">
+        <v>2022</v>
+      </c>
+      <c r="K2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>2022</v>
+      </c>
+      <c r="O2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3">
+        <v>125054</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
         <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>2022</v>
-      </c>
-      <c r="N2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
       </c>
       <c r="G3" t="s">
         <v>25</v>
       </c>
-      <c r="J3" t="s">
-        <v>28</v>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3">
+        <v>2023</v>
       </c>
       <c r="K3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" t="b">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>2021</v>
+      </c>
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4">
+        <v>87884</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
         <v>29</v>
       </c>
-      <c r="L3" t="b">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>2022</v>
-      </c>
-      <c r="N3" t="b">
-        <v>1</v>
+      <c r="I4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" t="b">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>2023</v>
+      </c>
+      <c r="O4" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:15">
+      <c r="A5">
+        <v>409236</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D5">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" t="b">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>2019</v>
-      </c>
-      <c r="N4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
+      <c r="E5">
+        <v>40</v>
       </c>
       <c r="F5" t="s">
         <v>21</v>
       </c>
       <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5">
+        <v>2023</v>
+      </c>
+      <c r="K5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>2021</v>
+      </c>
+      <c r="O5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6">
+        <v>47911</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6">
+        <v>1079</v>
+      </c>
+      <c r="E6">
+        <v>197</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
         <v>25</v>
       </c>
-      <c r="J5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="H6" t="s">
         <v>29</v>
       </c>
-      <c r="L5" t="b">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>2021</v>
-      </c>
-      <c r="N5" t="b">
-        <v>1</v>
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6">
+        <v>2023</v>
+      </c>
+      <c r="K6" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" t="s">
+        <v>41</v>
+      </c>
+      <c r="M6" t="b">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>2003</v>
+      </c>
+      <c r="O6" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
+    <row r="7" spans="1:15">
+      <c r="A7">
+        <v>393489</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
         <v>23</v>
-      </c>
-      <c r="G6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K6" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" t="b">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>2013</v>
-      </c>
-      <c r="N6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
       </c>
       <c r="G7" t="s">
         <v>25</v>
       </c>
-      <c r="J7" t="s">
-        <v>28</v>
+      <c r="H7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7">
+        <v>2023</v>
       </c>
       <c r="K7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L7" t="b">
-        <v>1</v>
-      </c>
-      <c r="M7">
-        <v>2021</v>
-      </c>
-      <c r="N7" t="b">
+        <v>35</v>
+      </c>
+      <c r="L7" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>2003</v>
+      </c>
+      <c r="O7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
+        <v>5884</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="E8" t="s">
-        <v>18</v>
+      <c r="E8">
+        <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8" t="s">
         <v>25</v>
       </c>
-      <c r="J8" t="s">
-        <v>28</v>
+      <c r="H8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8">
+        <v>2020</v>
       </c>
       <c r="K8" t="s">
-        <v>29</v>
-      </c>
-      <c r="L8" t="b">
-        <v>1</v>
-      </c>
-      <c r="M8">
+        <v>40</v>
+      </c>
+      <c r="L8" t="s">
+        <v>41</v>
+      </c>
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>2020</v>
+      </c>
+      <c r="O8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9">
+        <v>329892</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>137</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9">
         <v>2021</v>
       </c>
-      <c r="N8" t="b">
+      <c r="K9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" t="s">
+        <v>41</v>
+      </c>
+      <c r="M9" t="b">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>2009</v>
+      </c>
+      <c r="O9" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
+    <row r="10" spans="1:15">
+      <c r="A10">
+        <v>49195</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
         <v>18</v>
       </c>
-      <c r="F9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" t="s">
-        <v>28</v>
-      </c>
-      <c r="K9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" t="b">
-        <v>1</v>
-      </c>
-      <c r="M9">
-        <v>2021</v>
-      </c>
-      <c r="N9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
         <v>19</v>
-      </c>
-      <c r="F10" t="s">
-        <v>21</v>
       </c>
       <c r="G10" t="s">
         <v>25</v>
       </c>
-      <c r="J10" t="s">
+      <c r="H10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10">
+        <v>2020</v>
+      </c>
+      <c r="K10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" t="s">
+        <v>41</v>
+      </c>
+      <c r="M10" t="b">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>2017</v>
+      </c>
+      <c r="O10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11">
+        <v>298115</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>23</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" t="s">
         <v>28</v>
       </c>
-      <c r="K10" t="s">
-        <v>29</v>
-      </c>
-      <c r="L10" t="b">
-        <v>1</v>
-      </c>
-      <c r="M10">
-        <v>2019</v>
-      </c>
-      <c r="N10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" t="s">
-        <v>28</v>
+      <c r="H11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11">
+        <v>2023</v>
       </c>
       <c r="K11" t="s">
-        <v>29</v>
-      </c>
-      <c r="L11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M11">
+        <v>40</v>
+      </c>
+      <c r="L11" t="s">
+        <v>41</v>
+      </c>
+      <c r="M11" t="b">
+        <v>1</v>
+      </c>
+      <c r="N11">
         <v>2021</v>
       </c>
-      <c r="N11" t="b">
+      <c r="O11" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>